<commit_message>
update the draft manuscript
</commit_message>
<xml_diff>
--- a/tables/positive.xlsx
+++ b/tables/positive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yzl0084/Documents/Research/Lamellibrachia-genome/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD04F2F-AC7B-7149-84E4-626D77954463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BB6086-154B-5346-B3F0-A3A37243C636}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="28040" windowHeight="16100" xr2:uid="{48526DB9-ACDB-F948-871F-1983082C3FFF}"/>
   </bookViews>
@@ -1399,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F54D0A3-71A8-984C-8662-FE9C53D18D3D}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>